<commit_message>
Report Function Finished. Adjusting Summary Sheet Details
</commit_message>
<xml_diff>
--- a/Report_Temp.xlsx
+++ b/Report_Temp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="4965" windowWidth="24240" windowHeight="7680" tabRatio="693"/>
+    <workbookView xWindow="5715" yWindow="1725" windowWidth="24240" windowHeight="7620" tabRatio="693"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ToolVersion" sheetId="22896" state="hidden" r:id="rId10"/>
     <sheet name="ProcedureVersion" sheetId="22903" state="hidden" r:id="rId11"/>
     <sheet name="Result Matrix" sheetId="22904" state="hidden" r:id="rId12"/>
+    <sheet name="Report" sheetId="22905" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_context">defaultValues!$F$3:$F$4</definedName>
@@ -89,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="588">
   <si>
     <t>Regression thread</t>
   </si>
@@ -1877,6 +1878,36 @@
   <si>
     <t>TAT</t>
   </si>
+  <si>
+    <t>Attribute_Description(MCS)</t>
+  </si>
+  <si>
+    <t>DC_Data_Type</t>
+  </si>
+  <si>
+    <t>v0_label(0)</t>
+  </si>
+  <si>
+    <t>v0_Severity</t>
+  </si>
+  <si>
+    <t>v0_State</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Eqpt_Description(MCS)</t>
+  </si>
+  <si>
+    <t>Eqpt_Identifier</t>
+  </si>
+  <si>
+    <t>Register_Address/File</t>
+  </si>
+  <si>
+    <t>Bit_offset</t>
+  </si>
 </sst>
 </file>
 
@@ -1886,7 +1917,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2153,8 +2184,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="58">
+  <fills count="61">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2495,6 +2539,24 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray0625">
+        <fgColor indexed="22"/>
+        <bgColor indexed="41"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray0625">
+        <fgColor indexed="22"/>
+        <bgColor indexed="42"/>
       </patternFill>
     </fill>
   </fills>
@@ -3236,7 +3298,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="248">
+  <cellXfs count="256">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3759,6 +3821,30 @@
     <xf numFmtId="0" fontId="0" fillId="48" borderId="10" xfId="47" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="58" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="59" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="60" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="52" borderId="50" xfId="43" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="52" borderId="10" xfId="43" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="48" borderId="10" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="46" borderId="10" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="50" borderId="46" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3879,6 +3965,21 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="23" xfId="34" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3888,41 +3989,26 @@
     <xf numFmtId="0" fontId="18" fillId="32" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="44" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="44" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="25" xfId="34" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="26" xfId="34" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="44" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="44" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3985,7 +4071,95 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="41"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="31"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="49"/>
+          <bgColor indexed="11"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -4160,6 +4334,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4296,6 +4471,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5744,8 +5920,8 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6007,11 +6183,11 @@
       <c r="A15" s="138"/>
       <c r="B15" s="141"/>
       <c r="C15" s="138"/>
-      <c r="D15" s="190"/>
-      <c r="E15" s="191"/>
+      <c r="D15" s="198"/>
+      <c r="E15" s="199"/>
       <c r="F15" s="149"/>
-      <c r="G15" s="190"/>
-      <c r="H15" s="191"/>
+      <c r="G15" s="198"/>
+      <c r="H15" s="199"/>
       <c r="I15" s="138"/>
       <c r="J15" s="139"/>
     </row>
@@ -6214,8 +6390,8 @@
       </c>
       <c r="E26" s="159"/>
       <c r="F26" s="149"/>
-      <c r="G26" s="192"/>
-      <c r="H26" s="193"/>
+      <c r="G26" s="200"/>
+      <c r="H26" s="201"/>
       <c r="I26" s="138"/>
       <c r="J26" s="139"/>
     </row>
@@ -6229,8 +6405,8 @@
       </c>
       <c r="E27" s="155"/>
       <c r="F27" s="149"/>
-      <c r="G27" s="194"/>
-      <c r="H27" s="195"/>
+      <c r="G27" s="202"/>
+      <c r="H27" s="203"/>
       <c r="I27" s="143"/>
       <c r="J27" s="139"/>
     </row>
@@ -6243,8 +6419,8 @@
       </c>
       <c r="E28" s="155"/>
       <c r="F28" s="149"/>
-      <c r="G28" s="196"/>
-      <c r="H28" s="197"/>
+      <c r="G28" s="204"/>
+      <c r="H28" s="205"/>
       <c r="I28" s="143"/>
       <c r="J28" s="139"/>
     </row>
@@ -6290,8 +6466,8 @@
       </c>
       <c r="E31" s="155"/>
       <c r="F31" s="149"/>
-      <c r="G31" s="198"/>
-      <c r="H31" s="199"/>
+      <c r="G31" s="206"/>
+      <c r="H31" s="207"/>
       <c r="I31" s="143"/>
       <c r="J31" s="139"/>
     </row>
@@ -6303,10 +6479,13 @@
         <f>Language!$D$56</f>
         <v>Test case result</v>
       </c>
-      <c r="E32" s="156"/>
+      <c r="E32" s="156">
+        <f>SUM(E26:E31)</f>
+        <v>0</v>
+      </c>
       <c r="F32" s="149"/>
-      <c r="G32" s="200"/>
-      <c r="H32" s="201"/>
+      <c r="G32" s="208"/>
+      <c r="H32" s="209"/>
       <c r="I32" s="143"/>
       <c r="J32" s="139"/>
     </row>
@@ -6444,19 +6623,19 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"not testable"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"out of scope"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"passed with comment"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7298,14 +7477,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="C1" s="245" t="s">
+      <c r="C1" s="253" t="s">
         <v>512</v>
       </c>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
+      <c r="D1" s="253"/>
+      <c r="E1" s="253"/>
+      <c r="F1" s="253"/>
+      <c r="G1" s="253"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" s="123" t="s">
@@ -7328,7 +7507,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="246" t="s">
+      <c r="A3" s="254" t="s">
         <v>513</v>
       </c>
       <c r="B3" s="129" t="s">
@@ -7354,7 +7533,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="246"/>
+      <c r="A4" s="254"/>
       <c r="B4" s="132" t="s">
         <v>30</v>
       </c>
@@ -7378,27 +7557,27 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="246"/>
+      <c r="A5" s="254"/>
       <c r="B5" s="129" t="s">
         <v>515</v>
       </c>
       <c r="C5" s="130" t="s">
         <v>514</v>
       </c>
-      <c r="D5" s="247" t="s">
+      <c r="D5" s="255" t="s">
         <v>516</v>
       </c>
-      <c r="E5" s="247"/>
+      <c r="E5" s="255"/>
       <c r="F5" s="130">
         <v>0</v>
       </c>
-      <c r="G5" s="247" t="s">
+      <c r="G5" s="255" t="s">
         <v>516</v>
       </c>
-      <c r="H5" s="247"/>
+      <c r="H5" s="255"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="246"/>
+      <c r="A6" s="254"/>
       <c r="B6" s="133" t="s">
         <v>517</v>
       </c>
@@ -7422,7 +7601,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="246"/>
+      <c r="A7" s="254"/>
       <c r="B7" s="134" t="s">
         <v>284</v>
       </c>
@@ -7446,7 +7625,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="246"/>
+      <c r="A8" s="254"/>
       <c r="B8" s="135" t="s">
         <v>160</v>
       </c>
@@ -7470,7 +7649,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="246"/>
+      <c r="A9" s="254"/>
       <c r="B9" s="136" t="s">
         <v>22</v>
       </c>
@@ -7526,6 +7705,116 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="122" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="193" t="s">
+        <v>583</v>
+      </c>
+      <c r="B1" s="193" t="s">
+        <v>584</v>
+      </c>
+      <c r="C1" s="192" t="s">
+        <v>585</v>
+      </c>
+      <c r="D1" s="190" t="s">
+        <v>578</v>
+      </c>
+      <c r="E1" s="191" t="s">
+        <v>579</v>
+      </c>
+      <c r="F1" s="192" t="s">
+        <v>580</v>
+      </c>
+      <c r="G1" s="193" t="s">
+        <v>581</v>
+      </c>
+      <c r="H1" s="193" t="s">
+        <v>582</v>
+      </c>
+      <c r="I1" s="193" t="s">
+        <v>586</v>
+      </c>
+      <c r="J1" s="193" t="s">
+        <v>587</v>
+      </c>
+      <c r="K1" s="194" t="s">
+        <v>354</v>
+      </c>
+      <c r="L1" s="195" t="s">
+        <v>356</v>
+      </c>
+      <c r="M1" s="195" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="195" t="s">
+        <v>264</v>
+      </c>
+      <c r="O1" s="195" t="s">
+        <v>162</v>
+      </c>
+      <c r="P1" s="195" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K2" s="196" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="197"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
+      <c r="Q3" s="122"/>
+      <c r="R3" s="122"/>
+      <c r="S3" s="122"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"OS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"NT"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"OKWC"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"NOK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
+      <formula>$B2="X"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="7" stopIfTrue="1">
+      <formula>NOT(ISERROR(SEARCH("P",$B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7550,16 +7839,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="202" t="s">
+      <c r="B3" s="210" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="210"/>
+      <c r="G3" s="210"/>
+      <c r="H3" s="210"/>
+      <c r="I3" s="210"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -7878,11 +8167,11 @@
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="207" t="s">
+      <c r="C4" s="215" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="207"/>
-      <c r="E4" s="207"/>
+      <c r="D4" s="215"/>
+      <c r="E4" s="215"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -7899,7 +8188,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="203" t="s">
+      <c r="B7" s="211" t="s">
         <v>481</v>
       </c>
       <c r="C7" s="118" t="s">
@@ -7913,7 +8202,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="204"/>
+      <c r="B8" s="212"/>
       <c r="C8" s="118" t="s">
         <v>160</v>
       </c>
@@ -7925,7 +8214,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="204"/>
+      <c r="B9" s="212"/>
       <c r="C9" s="118" t="s">
         <v>284</v>
       </c>
@@ -7937,7 +8226,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="204"/>
+      <c r="B10" s="212"/>
       <c r="C10" s="118" t="s">
         <v>29</v>
       </c>
@@ -7949,7 +8238,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="205"/>
+      <c r="B11" s="213"/>
       <c r="C11" s="118" t="s">
         <v>30</v>
       </c>
@@ -7961,7 +8250,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="203" t="s">
+      <c r="B12" s="211" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="118" t="s">
@@ -7975,7 +8264,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="205"/>
+      <c r="B13" s="213"/>
       <c r="C13" s="118" t="s">
         <v>96</v>
       </c>
@@ -7987,7 +8276,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="208" t="s">
+      <c r="B14" s="216" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="118" t="s">
@@ -8001,7 +8290,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="209"/>
+      <c r="B15" s="217"/>
       <c r="C15" s="118" t="s">
         <v>27</v>
       </c>
@@ -8013,7 +8302,7 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="206" t="s">
+      <c r="B16" s="214" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="118" t="s">
@@ -8027,7 +8316,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="206"/>
+      <c r="B17" s="214"/>
       <c r="C17" s="118" t="s">
         <v>359</v>
       </c>
@@ -8039,7 +8328,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="206"/>
+      <c r="B18" s="214"/>
       <c r="C18" s="118" t="s">
         <v>31</v>
       </c>
@@ -8051,7 +8340,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="206" t="s">
+      <c r="B19" s="214" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="119" t="s">
@@ -8065,7 +8354,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="206"/>
+      <c r="B20" s="214"/>
       <c r="C20" s="119" t="s">
         <v>359</v>
       </c>
@@ -8077,7 +8366,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="206"/>
+      <c r="B21" s="214"/>
       <c r="C21" s="119" t="s">
         <v>360</v>
       </c>
@@ -8089,7 +8378,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="203" t="s">
+      <c r="B22" s="211" t="s">
         <v>474</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -8103,7 +8392,7 @@
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="204"/>
+      <c r="B23" s="212"/>
       <c r="C23" s="3" t="s">
         <v>476</v>
       </c>
@@ -8115,7 +8404,7 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="204"/>
+      <c r="B24" s="212"/>
       <c r="C24" s="3" t="s">
         <v>477</v>
       </c>
@@ -8127,7 +8416,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="205"/>
+      <c r="B25" s="213"/>
       <c r="C25" s="3" t="s">
         <v>478</v>
       </c>
@@ -8139,7 +8428,7 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="203" t="s">
+      <c r="B26" s="211" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -8153,7 +8442,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="204"/>
+      <c r="B27" s="212"/>
       <c r="C27" s="3" t="s">
         <v>325</v>
       </c>
@@ -8165,7 +8454,7 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="204"/>
+      <c r="B28" s="212"/>
       <c r="C28" s="3" t="s">
         <v>362</v>
       </c>
@@ -8177,7 +8466,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="204"/>
+      <c r="B29" s="212"/>
       <c r="C29" s="3" t="s">
         <v>326</v>
       </c>
@@ -8189,7 +8478,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="205"/>
+      <c r="B30" s="213"/>
       <c r="C30" s="3" t="s">
         <v>363</v>
       </c>
@@ -10707,73 +10996,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="29" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="224" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
-      <c r="H1" s="217"/>
-      <c r="I1" s="218"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
+      <c r="F1" s="225"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
+      <c r="I1" s="226"/>
     </row>
     <row r="2" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="219" t="s">
+      <c r="A3" s="227" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="220"/>
-      <c r="C3" s="220"/>
-      <c r="D3" s="220"/>
-      <c r="E3" s="220"/>
-      <c r="F3" s="220"/>
-      <c r="G3" s="220"/>
-      <c r="H3" s="220"/>
-      <c r="I3" s="221"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="229"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="222"/>
-      <c r="I4" s="223"/>
+      <c r="B4" s="230"/>
+      <c r="C4" s="230"/>
+      <c r="D4" s="230"/>
+      <c r="E4" s="230"/>
+      <c r="F4" s="230"/>
+      <c r="G4" s="230"/>
+      <c r="H4" s="230"/>
+      <c r="I4" s="231"/>
     </row>
     <row r="5" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="225"/>
-      <c r="D5" s="225"/>
-      <c r="E5" s="225"/>
-      <c r="F5" s="225"/>
-      <c r="G5" s="225"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="226"/>
+      <c r="B5" s="232"/>
+      <c r="C5" s="233"/>
+      <c r="D5" s="233"/>
+      <c r="E5" s="233"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="233"/>
+      <c r="H5" s="233"/>
+      <c r="I5" s="234"/>
     </row>
     <row r="6" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J6" s="68"/>
     </row>
     <row r="7" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="227" t="s">
+      <c r="A7" s="235" t="s">
         <v>236</v>
       </c>
-      <c r="B7" s="228"/>
-      <c r="C7" s="228"/>
-      <c r="D7" s="228"/>
-      <c r="E7" s="228"/>
-      <c r="F7" s="228"/>
-      <c r="G7" s="228"/>
-      <c r="H7" s="228"/>
-      <c r="I7" s="229"/>
+      <c r="B7" s="236"/>
+      <c r="C7" s="236"/>
+      <c r="D7" s="236"/>
+      <c r="E7" s="236"/>
+      <c r="F7" s="236"/>
+      <c r="G7" s="236"/>
+      <c r="H7" s="236"/>
+      <c r="I7" s="237"/>
     </row>
     <row r="8" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
@@ -10916,32 +11205,32 @@
     </row>
     <row r="19" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="227" t="s">
+      <c r="A20" s="235" t="s">
         <v>182</v>
       </c>
-      <c r="B20" s="228"/>
-      <c r="C20" s="228"/>
-      <c r="D20" s="228"/>
-      <c r="E20" s="228"/>
-      <c r="F20" s="228"/>
-      <c r="G20" s="228"/>
-      <c r="H20" s="228"/>
-      <c r="I20" s="229"/>
+      <c r="B20" s="236"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
+      <c r="E20" s="236"/>
+      <c r="F20" s="236"/>
+      <c r="G20" s="236"/>
+      <c r="H20" s="236"/>
+      <c r="I20" s="237"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="210" t="s">
+      <c r="A21" s="218" t="s">
         <v>216</v>
       </c>
-      <c r="B21" s="211"/>
-      <c r="C21" s="211"/>
-      <c r="D21" s="211"/>
-      <c r="E21" s="212"/>
-      <c r="F21" s="213" t="s">
+      <c r="B21" s="219"/>
+      <c r="C21" s="219"/>
+      <c r="D21" s="219"/>
+      <c r="E21" s="220"/>
+      <c r="F21" s="221" t="s">
         <v>218</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="215"/>
+      <c r="G21" s="222"/>
+      <c r="H21" s="222"/>
+      <c r="I21" s="223"/>
     </row>
     <row r="22" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
@@ -11138,71 +11427,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="224" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
-      <c r="H1" s="217"/>
-      <c r="I1" s="218"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
+      <c r="F1" s="225"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
+      <c r="I1" s="226"/>
     </row>
     <row r="2" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="219" t="s">
+      <c r="A3" s="227" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="220"/>
-      <c r="C3" s="220"/>
-      <c r="D3" s="220"/>
-      <c r="E3" s="220"/>
-      <c r="F3" s="220"/>
-      <c r="G3" s="220"/>
-      <c r="H3" s="220"/>
-      <c r="I3" s="221"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="229"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="222"/>
-      <c r="I4" s="223"/>
+      <c r="B4" s="230"/>
+      <c r="C4" s="230"/>
+      <c r="D4" s="230"/>
+      <c r="E4" s="230"/>
+      <c r="F4" s="230"/>
+      <c r="G4" s="230"/>
+      <c r="H4" s="230"/>
+      <c r="I4" s="231"/>
     </row>
     <row r="5" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="230"/>
-      <c r="C5" s="231"/>
-      <c r="D5" s="231"/>
-      <c r="E5" s="231"/>
-      <c r="F5" s="231"/>
-      <c r="G5" s="231"/>
-      <c r="H5" s="231"/>
-      <c r="I5" s="232"/>
+      <c r="B5" s="243"/>
+      <c r="C5" s="244"/>
+      <c r="D5" s="244"/>
+      <c r="E5" s="244"/>
+      <c r="F5" s="244"/>
+      <c r="G5" s="244"/>
+      <c r="H5" s="244"/>
+      <c r="I5" s="245"/>
     </row>
     <row r="6" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="227" t="s">
+      <c r="A7" s="235" t="s">
         <v>195</v>
       </c>
-      <c r="B7" s="228"/>
-      <c r="C7" s="228"/>
-      <c r="D7" s="228"/>
-      <c r="E7" s="228"/>
-      <c r="F7" s="228"/>
-      <c r="G7" s="228"/>
-      <c r="H7" s="228"/>
-      <c r="I7" s="229"/>
+      <c r="B7" s="236"/>
+      <c r="C7" s="236"/>
+      <c r="D7" s="236"/>
+      <c r="E7" s="236"/>
+      <c r="F7" s="236"/>
+      <c r="G7" s="236"/>
+      <c r="H7" s="236"/>
+      <c r="I7" s="237"/>
     </row>
     <row r="8" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
@@ -11382,32 +11671,32 @@
     </row>
     <row r="19" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="227" t="s">
+      <c r="A20" s="235" t="s">
         <v>182</v>
       </c>
-      <c r="B20" s="228"/>
-      <c r="C20" s="228"/>
-      <c r="D20" s="228"/>
-      <c r="E20" s="228"/>
-      <c r="F20" s="228"/>
-      <c r="G20" s="228"/>
-      <c r="H20" s="228"/>
-      <c r="I20" s="229"/>
+      <c r="B20" s="236"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
+      <c r="E20" s="236"/>
+      <c r="F20" s="236"/>
+      <c r="G20" s="236"/>
+      <c r="H20" s="236"/>
+      <c r="I20" s="237"/>
     </row>
     <row r="21" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="237" t="s">
+      <c r="A21" s="242" t="s">
         <v>278</v>
       </c>
-      <c r="B21" s="211"/>
-      <c r="C21" s="211"/>
-      <c r="D21" s="211"/>
-      <c r="E21" s="212"/>
-      <c r="F21" s="213" t="s">
+      <c r="B21" s="219"/>
+      <c r="C21" s="219"/>
+      <c r="D21" s="219"/>
+      <c r="E21" s="220"/>
+      <c r="F21" s="221" t="s">
         <v>218</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="215"/>
+      <c r="G21" s="222"/>
+      <c r="H21" s="222"/>
+      <c r="I21" s="223"/>
       <c r="V21" s="56"/>
     </row>
     <row r="22" spans="1:22" s="37" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -11796,32 +12085,32 @@
     </row>
     <row r="35" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="227" t="s">
+      <c r="A36" s="235" t="s">
         <v>181</v>
       </c>
-      <c r="B36" s="228"/>
-      <c r="C36" s="228"/>
-      <c r="D36" s="228"/>
-      <c r="E36" s="228"/>
-      <c r="F36" s="228"/>
-      <c r="G36" s="228"/>
-      <c r="H36" s="228"/>
-      <c r="I36" s="229"/>
+      <c r="B36" s="236"/>
+      <c r="C36" s="236"/>
+      <c r="D36" s="236"/>
+      <c r="E36" s="236"/>
+      <c r="F36" s="236"/>
+      <c r="G36" s="236"/>
+      <c r="H36" s="236"/>
+      <c r="I36" s="237"/>
     </row>
     <row r="37" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="233" t="s">
+      <c r="A37" s="238" t="s">
         <v>189</v>
       </c>
-      <c r="B37" s="234"/>
-      <c r="C37" s="234"/>
-      <c r="D37" s="234"/>
-      <c r="E37" s="235"/>
-      <c r="F37" s="236" t="s">
+      <c r="B37" s="239"/>
+      <c r="C37" s="239"/>
+      <c r="D37" s="239"/>
+      <c r="E37" s="240"/>
+      <c r="F37" s="241" t="s">
         <v>218</v>
       </c>
-      <c r="G37" s="214"/>
-      <c r="H37" s="214"/>
-      <c r="I37" s="215"/>
+      <c r="G37" s="222"/>
+      <c r="H37" s="222"/>
+      <c r="I37" s="223"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="105" t="s">
@@ -12176,17 +12465,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A21:E21"/>
     <mergeCell ref="A20:I20"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A21:E21"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B18">
@@ -12261,44 +12550,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="224" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
-      <c r="H1" s="217"/>
-      <c r="I1" s="218"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
+      <c r="F1" s="225"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
+      <c r="I1" s="226"/>
     </row>
     <row r="2" spans="1:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="219" t="s">
+      <c r="A3" s="227" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="220"/>
-      <c r="C3" s="220"/>
-      <c r="D3" s="220"/>
-      <c r="E3" s="220"/>
-      <c r="F3" s="220"/>
-      <c r="G3" s="220"/>
-      <c r="H3" s="220"/>
-      <c r="I3" s="221"/>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="229"/>
     </row>
     <row r="4" spans="1:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="86" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="240"/>
-      <c r="C4" s="240"/>
-      <c r="D4" s="240"/>
-      <c r="E4" s="240"/>
-      <c r="F4" s="240"/>
-      <c r="G4" s="240"/>
-      <c r="H4" s="240"/>
-      <c r="I4" s="241"/>
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="252"/>
     </row>
     <row r="5" spans="1:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -12324,10 +12613,10 @@
       <c r="R6" s="187"/>
       <c r="S6" s="187"/>
       <c r="T6" s="188"/>
-      <c r="U6" s="242" t="s">
+      <c r="U6" s="246" t="s">
         <v>288</v>
       </c>
-      <c r="V6" s="243"/>
+      <c r="V6" s="247"/>
       <c r="W6" s="81"/>
       <c r="X6" s="81"/>
       <c r="Y6" s="81"/>
@@ -14196,32 +14485,32 @@
       <c r="X57" s="81"/>
     </row>
     <row r="58" spans="1:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="227" t="s">
+      <c r="A58" s="235" t="s">
         <v>182</v>
       </c>
-      <c r="B58" s="228"/>
-      <c r="C58" s="228"/>
-      <c r="D58" s="228"/>
-      <c r="E58" s="228"/>
-      <c r="F58" s="228"/>
-      <c r="G58" s="228"/>
-      <c r="H58" s="228"/>
-      <c r="I58" s="229"/>
+      <c r="B58" s="236"/>
+      <c r="C58" s="236"/>
+      <c r="D58" s="236"/>
+      <c r="E58" s="236"/>
+      <c r="F58" s="236"/>
+      <c r="G58" s="236"/>
+      <c r="H58" s="236"/>
+      <c r="I58" s="237"/>
     </row>
     <row r="59" spans="1:34" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="210" t="s">
+      <c r="A59" s="218" t="s">
         <v>189</v>
       </c>
-      <c r="B59" s="211"/>
-      <c r="C59" s="211"/>
-      <c r="D59" s="211"/>
-      <c r="E59" s="239"/>
-      <c r="F59" s="238" t="s">
+      <c r="B59" s="219"/>
+      <c r="C59" s="219"/>
+      <c r="D59" s="219"/>
+      <c r="E59" s="249"/>
+      <c r="F59" s="250" t="s">
         <v>187</v>
       </c>
-      <c r="G59" s="214"/>
-      <c r="H59" s="214"/>
-      <c r="I59" s="215"/>
+      <c r="G59" s="222"/>
+      <c r="H59" s="222"/>
+      <c r="I59" s="223"/>
     </row>
     <row r="60" spans="1:34" s="37" customFormat="1" ht="26.25" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="47" t="s">
@@ -14515,32 +14804,32 @@
     </row>
     <row r="72" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="227" t="s">
+      <c r="A73" s="235" t="s">
         <v>181</v>
       </c>
-      <c r="B73" s="228"/>
-      <c r="C73" s="228"/>
-      <c r="D73" s="228"/>
-      <c r="E73" s="228"/>
-      <c r="F73" s="228"/>
-      <c r="G73" s="228"/>
-      <c r="H73" s="228"/>
-      <c r="I73" s="229"/>
+      <c r="B73" s="236"/>
+      <c r="C73" s="236"/>
+      <c r="D73" s="236"/>
+      <c r="E73" s="236"/>
+      <c r="F73" s="236"/>
+      <c r="G73" s="236"/>
+      <c r="H73" s="236"/>
+      <c r="I73" s="237"/>
     </row>
     <row r="74" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="244" t="s">
+      <c r="A74" s="248" t="s">
         <v>189</v>
       </c>
-      <c r="B74" s="211"/>
-      <c r="C74" s="211"/>
-      <c r="D74" s="211"/>
-      <c r="E74" s="239"/>
-      <c r="F74" s="238" t="s">
+      <c r="B74" s="219"/>
+      <c r="C74" s="219"/>
+      <c r="D74" s="219"/>
+      <c r="E74" s="249"/>
+      <c r="F74" s="250" t="s">
         <v>187</v>
       </c>
-      <c r="G74" s="214"/>
-      <c r="H74" s="214"/>
-      <c r="I74" s="215"/>
+      <c r="G74" s="222"/>
+      <c r="H74" s="222"/>
+      <c r="I74" s="223"/>
     </row>
     <row r="75" spans="1:9" ht="26.25" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="40" t="s">
@@ -14628,16 +14917,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="B4:I4"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="A74:E74"/>
     <mergeCell ref="F74:I74"/>
     <mergeCell ref="A58:I58"/>
     <mergeCell ref="A73:I73"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="B4:I4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61:B71 B76:B80">

</xml_diff>